<commit_message>
restructure the file dir
</commit_message>
<xml_diff>
--- a/herbarium label/DARWIN_CORE_DB_SAVE/darwin_core_database.xlsx
+++ b/herbarium label/DARWIN_CORE_DB_SAVE/darwin_core_database.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t xml:space="preserve">GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -137,280 +137,220 @@
     <t xml:space="preserve">Kadoorie Farm &amp; Botanic Garden Herbarium (KFBG)</t>
   </si>
   <si>
-    <t xml:space="preserve">Caroline Law Man Yee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL0385</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-11-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">毛排錢草</t>
+    <t xml:space="preserve">Kelvin Ip Ka Lok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KI0227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-01-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海紅豆</t>
   </si>
   <si>
     <t xml:space="preserve">Fabaceae</t>
   </si>
   <si>
-    <t xml:space="preserve">Phyllodium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">elegans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Lour.) Desv.</t>
+    <t xml:space="preserve">Adenanthera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">microsperma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teijsm. &amp; Binnend.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">var.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Teijsm. et Binnend.) Nielsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hong Kong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Territories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tai Po</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tong Min Tsuen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS04, WP568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebe Lo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-09-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KI036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-01-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">胡桐</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clusiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calophyllum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membranaceum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardn. &amp; Champ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tsuen Wan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shing Mun Fung Shui Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Gale, Hon Cheuk Hei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KI252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-02-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">常綠臭椿</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simaroubaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ailanthus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fordii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nooteboom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lantau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nei Lak Shan, Lantau Peak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seedlet accession no. 8628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jinlong Zhang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JL0520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-01-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岗柃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pentaphylacaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eurya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groffii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merr.</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">Hong Kong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Territories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HO PUI RESERVOIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30.53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The specimen was collected by Dr. Charlotte Shiu's team under the name of Dr. Caroline Law Man Yee. GPS#04, WayPoint 732</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jinlong Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-11-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL0386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">葫蘆茶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tadehagi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">triquetrum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(L.) Ohashi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The specimen was collected by Dr. Charlotte Shiu's team under the name of Dr. Caroline Law Man Yee. GPS#04, WayPoint 733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL0387</t>
-  </si>
-  <si>
-    <t xml:space="preserve">石斑木</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rosaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rhaphiolepis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(L.) Lindl.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The specimen was collected by Dr. Charlotte Shiu's team under the name of Dr. Caroline Law Man Yee. GPS#04, WayPoint 734. Photo number 1050-1054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wang X. W.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S. E. S. Jones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">381</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1992-01-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">海金沙</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lygodiaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lygodium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">japonicum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Thunb.) Sw.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tai Po</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ng Tung Chai walk between Bottom Fall at " TMS " signpost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herb, 0.5m tall.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geographical Coordinates was estimated from Google Earth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wang X.W.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-07-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">954</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1992-10-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">大头茶</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gordonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">axillaris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dietr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadoorie Farm and Botanic Garden. Between Orchid Path , on slope above TS Woo Memorial Pavilion.</t>
+    <t xml:space="preserve">Tree Planting Site of Kadoorie Farm and Botanic Garden</t>
   </si>
   <si>
     <t xml:space="preserve">25</t>
   </si>
   <si>
-    <t xml:space="preserve">30.08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">503</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shrub 1.5m tall.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growing in mountain grassland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012-06-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1993-09-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">念珠藤</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apocynaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alyxia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sinensis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Champ. ex Benth.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadoorie Farm and Botanic Garden, N slop of Kwun Yam Shan near Enkianthus Walk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">480</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1993-9-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011-05-20</t>
+    <t xml:space="preserve">19.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree, 5m tall</t>
   </si>
 </sst>
 </file>
@@ -899,65 +839,73 @@
         <v>49</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2"/>
+        <v>53</v>
+      </c>
+      <c r="S2" t="s">
+        <v>54</v>
+      </c>
       <c r="T2"/>
       <c r="U2"/>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="X2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Y2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AB2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AC2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AE2"/>
       <c r="AF2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2"/>
+        <v>64</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>65</v>
+      </c>
       <c r="AH2"/>
       <c r="AI2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="AJ2" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
+      <c r="AL2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>67</v>
+      </c>
       <c r="AN2"/>
     </row>
     <row r="3">
@@ -971,89 +919,89 @@
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" t="s">
-        <v>49</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
       <c r="P3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3"/>
+        <v>75</v>
+      </c>
+      <c r="S3" t="s">
+        <v>76</v>
+      </c>
       <c r="T3"/>
       <c r="U3"/>
       <c r="V3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W3" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="X3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="Y3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA3" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="AB3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AC3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="AE3"/>
-      <c r="AF3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG3"/>
+      <c r="AF3"/>
+      <c r="AG3" t="s">
+        <v>65</v>
+      </c>
       <c r="AH3"/>
       <c r="AI3" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="AJ3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
+      <c r="AL3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>67</v>
+      </c>
       <c r="AN3"/>
     </row>
     <row r="4">
@@ -1065,91 +1013,93 @@
       <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="E4"/>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="K4" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>49</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
       <c r="P4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4"/>
+        <v>90</v>
+      </c>
+      <c r="S4" t="s">
+        <v>91</v>
+      </c>
       <c r="T4"/>
       <c r="U4"/>
       <c r="V4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W4" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="X4" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="Y4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AB4" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="AC4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD4" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="AE4"/>
       <c r="AF4" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="AG4"/>
       <c r="AH4"/>
       <c r="AI4" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="AJ4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AK4"/>
-      <c r="AL4"/>
-      <c r="AM4"/>
+      <c r="AL4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>67</v>
+      </c>
       <c r="AN4"/>
     </row>
     <row r="5">
@@ -1159,89 +1109,91 @@
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K5" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="O5" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="P5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R5" t="s">
-        <v>52</v>
-      </c>
-      <c r="S5"/>
+        <v>53</v>
+      </c>
+      <c r="S5" t="s">
+        <v>106</v>
+      </c>
       <c r="T5"/>
       <c r="U5"/>
       <c r="V5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W5" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="X5" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="Y5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA5" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="AB5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="AC5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE5"/>
-      <c r="AF5" t="s">
-        <v>83</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF5"/>
       <c r="AG5"/>
       <c r="AH5"/>
       <c r="AI5" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="AJ5" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="AK5"/>
       <c r="AL5"/>
@@ -1255,101 +1207,95 @@
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" t="s">
-        <v>85</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="I6" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="J6" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="L6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="P6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R6" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="S6" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="T6"/>
       <c r="U6"/>
       <c r="V6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W6" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="X6" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="Y6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="AB6" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="AC6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD6" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AE6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>101</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="AF6"/>
       <c r="AG6"/>
       <c r="AH6"/>
       <c r="AI6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="AJ6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AK6"/>
       <c r="AL6"/>
-      <c r="AM6" t="s">
-        <v>104</v>
-      </c>
+      <c r="AM6"/>
       <c r="AN6"/>
     </row>
     <row r="7">
@@ -1359,202 +1305,96 @@
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>85</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E7"/>
       <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" t="s">
         <v>105</v>
       </c>
-      <c r="G7" t="s">
+      <c r="N7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7" t="s">
         <v>106</v>
-      </c>
-      <c r="H7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J7" t="s">
-        <v>109</v>
-      </c>
-      <c r="K7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" t="s">
-        <v>49</v>
-      </c>
-      <c r="P7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>51</v>
-      </c>
-      <c r="R7" t="s">
-        <v>93</v>
-      </c>
-      <c r="S7" t="s">
-        <v>112</v>
       </c>
       <c r="T7"/>
       <c r="U7"/>
       <c r="V7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="W7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="X7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="Y7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AA7" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="AB7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="AC7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AD7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="AE7" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>118</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="AF7"/>
       <c r="AG7"/>
       <c r="AH7"/>
       <c r="AI7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="AJ7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="AK7"/>
       <c r="AL7"/>
-      <c r="AM7" t="s">
-        <v>119</v>
-      </c>
+      <c r="AM7"/>
       <c r="AN7"/>
-    </row>
-    <row r="8">
-      <c r="A8"/>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I8" t="s">
-        <v>123</v>
-      </c>
-      <c r="J8" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" t="s">
-        <v>125</v>
-      </c>
-      <c r="L8" t="s">
-        <v>126</v>
-      </c>
-      <c r="M8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" t="s">
-        <v>49</v>
-      </c>
-      <c r="O8" t="s">
-        <v>49</v>
-      </c>
-      <c r="P8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" t="s">
-        <v>93</v>
-      </c>
-      <c r="S8" t="s">
-        <v>127</v>
-      </c>
-      <c r="T8"/>
-      <c r="U8"/>
-      <c r="V8" t="s">
-        <v>53</v>
-      </c>
-      <c r="W8" t="s">
-        <v>113</v>
-      </c>
-      <c r="X8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE8"/>
-      <c r="AF8"/>
-      <c r="AG8"/>
-      <c r="AH8"/>
-      <c r="AI8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK8"/>
-      <c r="AL8"/>
-      <c r="AM8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AN8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upgraded according to the change of herblabel
</commit_message>
<xml_diff>
--- a/herbarium label/DARWIN_CORE_DB_SAVE/darwin_core_database.xlsx
+++ b/herbarium label/DARWIN_CORE_DB_SAVE/darwin_core_database.xlsx
@@ -3,354 +3,372 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
-  <si>
-    <t xml:space="preserve">GLOBAL_UNIQUE_IDENTIFIER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HERBARIUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLLECTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADDITIONAL_COLLECTOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLLECTOR_NUMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_COLLECTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCAL_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FAMILY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPECIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTHOR_OF_SPECIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFRASPECIFIC_RANK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFRASPECIFIC_EPITHET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTHOR_OF_INFRASPECIFIC_RANK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATE_PROVINCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCALITY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMAGE_URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELATED_INFORMATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_DEGREE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_MINUTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_SECOND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAT_FLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_DEGREE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_MINUTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_SECOND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LON_FLAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELEVATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATTRIBUTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REMARKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GEOREFERENCE_SOURCES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDENTIFIED_BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_IDENTIFIED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPE_STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROCESSED_BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE_LASTMODIFIED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPECIMEN_LOCATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kadoorie Farm &amp; Botanic Garden Herbarium (KFBG)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kelvin Ip Ka Lok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KI0227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-01-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">海紅豆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fabaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adenanthera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">microsperma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teijsm. &amp; Binnend.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">var.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Teijsm. et Binnend.) Nielsen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hong Kong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Territories</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tai Po</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tong Min Tsuen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS04, WP568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hebe Lo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-09-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KI036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014-01-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">胡桐</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clusiaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calophyllum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">membranaceum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gardn. &amp; Champ.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tsuen Wan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shing Mun Fung Shui Wood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephen Gale, Hon Cheuk Hei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KI252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015-02-25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">常綠臭椿</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simaroubaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ailanthus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fordii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nooteboom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lantau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nei Lak Shan, Lantau Peak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">514</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seedlet accession no. 8628</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jinlong Zhang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JL0520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016-01-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">岗柃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pentaphylacaceae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eurya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">groffii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Tree Planting Site of Kadoorie Farm and Botanic Garden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tree, 5m tall</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+  <si>
+    <t>GLOBAL_UNIQUE_IDENTIFIER</t>
+  </si>
+  <si>
+    <t>HERBARIUM</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>COLLECTOR</t>
+  </si>
+  <si>
+    <t>ADDITIONAL_COLLECTOR</t>
+  </si>
+  <si>
+    <t>COLLECTOR_NUMBER</t>
+  </si>
+  <si>
+    <t>DATE_COLLECTED</t>
+  </si>
+  <si>
+    <t>LOCAL_NAME</t>
+  </si>
+  <si>
+    <t>FAMILY</t>
+  </si>
+  <si>
+    <t>GENUS</t>
+  </si>
+  <si>
+    <t>SPECIES</t>
+  </si>
+  <si>
+    <t>AUTHOR_OF_SPECIES</t>
+  </si>
+  <si>
+    <t>INFRASPECIFIC_RANK</t>
+  </si>
+  <si>
+    <t>INFRASPECIFIC_EPITHET</t>
+  </si>
+  <si>
+    <t>AUTHOR_OF_INFRASPECIFIC_RANK</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>STATE_PROVINCE</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>LOCALITY</t>
+  </si>
+  <si>
+    <t>IMAGE_URL</t>
+  </si>
+  <si>
+    <t>RELATED_INFORMATION</t>
+  </si>
+  <si>
+    <t>LAT_DEGREE</t>
+  </si>
+  <si>
+    <t>LAT_MINUTE</t>
+  </si>
+  <si>
+    <t>LAT_SECOND</t>
+  </si>
+  <si>
+    <t>LAT_FLAG</t>
+  </si>
+  <si>
+    <t>LON_DEGREE</t>
+  </si>
+  <si>
+    <t>LON_MINUTE</t>
+  </si>
+  <si>
+    <t>LON_SECOND</t>
+  </si>
+  <si>
+    <t>LON_FLAG</t>
+  </si>
+  <si>
+    <t>ELEVATION</t>
+  </si>
+  <si>
+    <t>ATTRIBUTES</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
+  </si>
+  <si>
+    <t>GEOREFERENCE_SOURCES</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>IDENTIFIED_BY</t>
+  </si>
+  <si>
+    <t>DATE_IDENTIFIED</t>
+  </si>
+  <si>
+    <t>TYPE_STATUS</t>
+  </si>
+  <si>
+    <t>PROCESSED_BY</t>
+  </si>
+  <si>
+    <t>DATE_LASTMODIFIED</t>
+  </si>
+  <si>
+    <t>SPECIMEN_LOCATION</t>
+  </si>
+  <si>
+    <t>Kadoorie Farm &amp; Botanic Garden Herbarium (KFBG)</t>
+  </si>
+  <si>
+    <t>Kelvin Ip Ka Lok</t>
+  </si>
+  <si>
+    <t>KI0227</t>
+  </si>
+  <si>
+    <t>2015-01-12</t>
+  </si>
+  <si>
+    <t>海紅豆</t>
+  </si>
+  <si>
+    <t>Fabaceae</t>
+  </si>
+  <si>
+    <t>Adenanthera</t>
+  </si>
+  <si>
+    <t>microsperma</t>
+  </si>
+  <si>
+    <t>Teijsm. &amp; Binnend.</t>
+  </si>
+  <si>
+    <t>var.</t>
+  </si>
+  <si>
+    <t>(Teijsm. et Binnend.) Nielsen</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>New Territories</t>
+  </si>
+  <si>
+    <t>Tai Po</t>
+  </si>
+  <si>
+    <t>Tong Min Tsuen</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>8.05</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>19.43</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>GPS04, WP568</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Hebe Lo</t>
+  </si>
+  <si>
+    <t>2015-09-02</t>
+  </si>
+  <si>
+    <t>KI036</t>
+  </si>
+  <si>
+    <t>2014-01-28</t>
+  </si>
+  <si>
+    <t>胡桐</t>
+  </si>
+  <si>
+    <t>Clusiaceae</t>
+  </si>
+  <si>
+    <t>Calophyllum</t>
+  </si>
+  <si>
+    <t>membranaceum</t>
+  </si>
+  <si>
+    <t>Gardn. &amp; Champ.</t>
+  </si>
+  <si>
+    <t>Tsuen Wan</t>
+  </si>
+  <si>
+    <t>Shing Mun Fung Shui Wood</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>48.9</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>Stephen Gale, Hon Cheuk Hei</t>
+  </si>
+  <si>
+    <t>KI252</t>
+  </si>
+  <si>
+    <t>2015-02-25</t>
+  </si>
+  <si>
+    <t>常綠臭椿</t>
+  </si>
+  <si>
+    <t>Simaroubaceae</t>
+  </si>
+  <si>
+    <t>Ailanthus</t>
+  </si>
+  <si>
+    <t>fordii</t>
+  </si>
+  <si>
+    <t>Nooteboom</t>
+  </si>
+  <si>
+    <t>Lantau</t>
+  </si>
+  <si>
+    <t>Nei Lak Shan, Lantau Peak</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>56.47</t>
+  </si>
+  <si>
+    <t>50.81</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>Seedlet accession no. 8628</t>
+  </si>
+  <si>
+    <t>Jinlong Zhang</t>
+  </si>
+  <si>
+    <t>嘉道理农场暨植物园</t>
+  </si>
+  <si>
+    <t>张金龙</t>
+  </si>
+  <si>
+    <t>JL0520</t>
+  </si>
+  <si>
+    <t>2016-01-18</t>
+  </si>
+  <si>
+    <t>岗柃</t>
+  </si>
+  <si>
+    <t>Pentaphylacaceae</t>
+  </si>
+  <si>
+    <t>Eurya</t>
+  </si>
+  <si>
+    <t>groffii</t>
+  </si>
+  <si>
+    <t>Merr.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>香港</t>
+  </si>
+  <si>
+    <t>新界</t>
+  </si>
+  <si>
+    <t>大埔</t>
+  </si>
+  <si>
+    <t>嘉道理农场植树区</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>19.49</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>25.99</t>
+  </si>
+  <si>
+    <t>603</t>
+  </si>
+  <si>
+    <t>Tree, 5m tall</t>
+  </si>
+  <si>
+    <t>Tree Planting Site of Kadoorie Farm and Botanic Garden</t>
   </si>
 </sst>
 </file>
@@ -1105,54 +1123,54 @@
     <row r="5">
       <c r="A5"/>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P5" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="Q5" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="R5" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="S5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="T5"/>
       <c r="U5"/>
@@ -1160,10 +1178,10 @@
         <v>55</v>
       </c>
       <c r="W5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="X5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="Y5" t="s">
         <v>58</v>
@@ -1172,28 +1190,28 @@
         <v>59</v>
       </c>
       <c r="AA5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AB5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AC5" t="s">
         <v>62</v>
       </c>
       <c r="AD5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AE5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="AF5"/>
       <c r="AG5"/>
       <c r="AH5"/>
       <c r="AI5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AJ5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AK5"/>
       <c r="AL5"/>
@@ -1203,54 +1221,54 @@
     <row r="6">
       <c r="A6"/>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="C6"/>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="M6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="Q6" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="R6" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="S6" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="T6"/>
       <c r="U6"/>
@@ -1258,10 +1276,10 @@
         <v>55</v>
       </c>
       <c r="W6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="X6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="Y6" t="s">
         <v>58</v>
@@ -1270,28 +1288,28 @@
         <v>59</v>
       </c>
       <c r="AA6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AB6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AC6" t="s">
         <v>62</v>
       </c>
       <c r="AD6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AE6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="AF6"/>
       <c r="AG6"/>
       <c r="AH6"/>
       <c r="AI6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AJ6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AK6"/>
       <c r="AL6"/>
@@ -1301,54 +1319,54 @@
     <row r="7">
       <c r="A7"/>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="M7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="N7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="O7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="R7" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="S7" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="T7"/>
       <c r="U7"/>
@@ -1356,10 +1374,10 @@
         <v>55</v>
       </c>
       <c r="W7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="X7" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="Y7" t="s">
         <v>58</v>
@@ -1368,33 +1386,621 @@
         <v>59</v>
       </c>
       <c r="AA7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AB7" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AC7" t="s">
         <v>62</v>
       </c>
       <c r="AD7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AE7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="AF7"/>
       <c r="AG7"/>
       <c r="AH7"/>
       <c r="AI7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AJ7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="AK7"/>
       <c r="AL7"/>
       <c r="AM7"/>
       <c r="AN7"/>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O8" t="s">
+        <v>107</v>
+      </c>
+      <c r="P8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" t="s">
+        <v>53</v>
+      </c>
+      <c r="S8" t="s">
+        <v>118</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" t="s">
+        <v>112</v>
+      </c>
+      <c r="X8" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" t="s">
+        <v>107</v>
+      </c>
+      <c r="O9" t="s">
+        <v>107</v>
+      </c>
+      <c r="P9" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>52</v>
+      </c>
+      <c r="R9" t="s">
+        <v>53</v>
+      </c>
+      <c r="S9" t="s">
+        <v>118</v>
+      </c>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9" t="s">
+        <v>55</v>
+      </c>
+      <c r="W9" t="s">
+        <v>112</v>
+      </c>
+      <c r="X9" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" t="s">
+        <v>106</v>
+      </c>
+      <c r="M10" t="s">
+        <v>107</v>
+      </c>
+      <c r="N10" t="s">
+        <v>107</v>
+      </c>
+      <c r="O10" t="s">
+        <v>107</v>
+      </c>
+      <c r="P10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R10" t="s">
+        <v>53</v>
+      </c>
+      <c r="S10" t="s">
+        <v>118</v>
+      </c>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10" t="s">
+        <v>55</v>
+      </c>
+      <c r="W10" t="s">
+        <v>112</v>
+      </c>
+      <c r="X10" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O11" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>52</v>
+      </c>
+      <c r="R11" t="s">
+        <v>53</v>
+      </c>
+      <c r="S11" t="s">
+        <v>118</v>
+      </c>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" t="s">
+        <v>112</v>
+      </c>
+      <c r="X11" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>106</v>
+      </c>
+      <c r="M12" t="s">
+        <v>107</v>
+      </c>
+      <c r="N12" t="s">
+        <v>107</v>
+      </c>
+      <c r="O12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" t="s">
+        <v>53</v>
+      </c>
+      <c r="S12" t="s">
+        <v>118</v>
+      </c>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12" t="s">
+        <v>55</v>
+      </c>
+      <c r="W12" t="s">
+        <v>112</v>
+      </c>
+      <c r="X12" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K13" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" t="s">
+        <v>106</v>
+      </c>
+      <c r="M13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" t="s">
+        <v>107</v>
+      </c>
+      <c r="O13" t="s">
+        <v>107</v>
+      </c>
+      <c r="P13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>52</v>
+      </c>
+      <c r="R13" t="s">
+        <v>53</v>
+      </c>
+      <c r="S13" t="s">
+        <v>118</v>
+      </c>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13" t="s">
+        <v>55</v>
+      </c>
+      <c r="W13" t="s">
+        <v>112</v>
+      </c>
+      <c r="X13" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>